<commit_message>
Added quality control checklist
</commit_message>
<xml_diff>
--- a/Etapa 2/Checklist Gerência de Projeto.xlsx
+++ b/Etapa 2/Checklist Gerência de Projeto.xlsx
@@ -678,21 +678,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -998,7 +998,7 @@
   <dimension ref="B1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1008,10 +1008,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="9"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
@@ -1026,52 +1026,52 @@
     </row>
     <row r="5" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="6" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="6" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="6" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="6" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="6"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="7" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1109,12 +1109,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1444,12 +1444,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1623,12 +1623,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1820,12 +1820,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1890,12 +1890,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1987,12 +1987,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -2185,12 +2185,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">

</xml_diff>